<commit_message>
Update các file liên quan đến dự án
</commit_message>
<xml_diff>
--- a/docs/Sprint 7 - 1905 To 0106/LogTime_sprint 7.xlsx
+++ b/docs/Sprint 7 - 1905 To 0106/LogTime_sprint 7.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14160" windowHeight="6165"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14160" windowHeight="6165" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ANLT" sheetId="1" r:id="rId1"/>
@@ -532,7 +532,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -542,8 +542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -682,6 +682,15 @@
       <c r="K9">
         <v>4</v>
       </c>
+      <c r="M9">
+        <v>4</v>
+      </c>
+      <c r="N9">
+        <v>10</v>
+      </c>
+      <c r="O9">
+        <v>6</v>
+      </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -738,15 +747,15 @@
       </c>
       <c r="M13">
         <f>SUM(Table2[30/05/2014])</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="N13">
         <f>SUM(Table2[31/05/2014])</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="O13">
         <f>SUM(Table2[01/06/2014])</f>
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -762,8 +771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R10"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -844,6 +853,12 @@
       <c r="F2">
         <v>3</v>
       </c>
+      <c r="L2">
+        <v>2</v>
+      </c>
+      <c r="O2">
+        <v>10</v>
+      </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -899,7 +914,7 @@
       </c>
       <c r="L10">
         <f>SUM(Table24[29/05/2014])</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M10">
         <f>SUM(Table24[30/05/2014])</f>
@@ -911,7 +926,7 @@
       </c>
       <c r="O10">
         <f>SUM(Table24[01/06/2014])</f>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>